<commit_message>
Adicionando a conexão ao Banco de dados
</commit_message>
<xml_diff>
--- a/ProjetoPooGrupo3/EscopoDB.xlsx
+++ b/ProjetoPooGrupo3/EscopoDB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programação\TICSerratec\POO\TrabalhoPOO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programação\SerraTEC\Programação Orientada a Objeto\ProjetoPooGrupo3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{98ED4C1D-AD8A-4B12-A29A-B59C573B1037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBA4BA1-3A14-4E88-9892-FFE81EAC8701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C4CD8D50-65E9-4A67-9AF4-43C64B912F79}"/>
+    <workbookView xWindow="35145" yWindow="7935" windowWidth="18030" windowHeight="10335" xr2:uid="{C4CD8D50-65E9-4A67-9AF4-43C64B912F79}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Cliente</t>
   </si>
@@ -66,12 +66,6 @@
     <t>qtdped</t>
   </si>
   <si>
-    <t>vlbruto</t>
-  </si>
-  <si>
-    <t>vlliq</t>
-  </si>
-  <si>
     <t>PedProd</t>
   </si>
   <si>
@@ -93,20 +87,49 @@
     <t>razaosocial</t>
   </si>
   <si>
-    <t>vldesc</t>
-  </si>
-  <si>
-    <t>vlacresc</t>
+    <t>pedido</t>
+  </si>
+  <si>
+    <t>produtos</t>
+  </si>
+  <si>
+    <t>pedidoitem</t>
+  </si>
+  <si>
+    <t>banana</t>
+  </si>
+  <si>
+    <t>maca</t>
+  </si>
+  <si>
+    <t>laranja</t>
+  </si>
+  <si>
+    <t>vl un</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -138,9 +161,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F6B670B-7913-4FCF-AE3C-4D93DBC627CE}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,13 +493,13 @@
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -484,13 +509,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
@@ -506,79 +531,140 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
         <v>12</v>
       </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" t="s">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H23" t="s">
         <v>22</v>
       </c>
-      <c r="G11" t="s">
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
         <v>23</v>
       </c>
-      <c r="H11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" t="s">
-        <v>21</v>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>2</v>
+      </c>
+      <c r="J24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26" t="s">
+        <v>25</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+      <c r="J26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H27">
+        <v>2</v>
+      </c>
+      <c r="I27">
+        <v>3</v>
+      </c>
+      <c r="J27">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>